<commit_message>
feat: hint  and constraint on tracing date (#372)
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/tracing_outcome.xlsx
+++ b/itech-malawi/forms/app/tracing_outcome.xlsx
@@ -1,28 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/itech-malawi/forms/app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8456943-42C1-6D43-A09B-DE518BBEC31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="survey" sheetId="1" r:id="rId4"/>
+    <sheet name="choices" sheetId="2" r:id="rId5"/>
+    <sheet name="settings" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
   <si>
     <t>type</t>
   </si>
@@ -222,13 +213,31 @@
     <t>Outcome: ${b2c_outcome}</t>
   </si>
   <si>
+    <t>select_one is_date_known</t>
+  </si>
+  <si>
+    <t>is_date_known</t>
+  </si>
+  <si>
+    <t>Is Date Known</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
     <t>date_of_event</t>
   </si>
   <si>
-    <t>Date of Event</t>
+    <t>Actual or Estimated Date of Event</t>
+  </si>
+  <si>
+    <t>${is_date_known} = 'yes'</t>
+  </si>
+  <si>
+    <t>.&lt;=date(today())</t>
+  </si>
+  <si>
+    <t>Value must be current or previous date</t>
   </si>
   <si>
     <t>formatted_doe</t>
@@ -315,10 +324,16 @@
     <t>Back To Care Outcome: ${b2c_outcome}</t>
   </si>
   <si>
+    <t>_is_date_known</t>
+  </si>
+  <si>
+    <t>Is Date Known: ${is_date_known}</t>
+  </si>
+  <si>
     <t>_date_of_event</t>
   </si>
   <si>
-    <t>Date of Event: ${formatted_doe}</t>
+    <t>Actual or Estimated Date of Event: ${formatted_doe}</t>
   </si>
   <si>
     <t>list_name</t>
@@ -375,6 +390,15 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -415,85 +439,60 @@
   </si>
   <si>
     <t>en</t>
-  </si>
-  <si>
-    <t>is_date_known</t>
-  </si>
-  <si>
-    <t>select_one is_date_known</t>
-  </si>
-  <si>
-    <t>Is Date Known</t>
-  </si>
-  <si>
-    <t>${is_date_known} = 'yes'</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>_is_date_known</t>
-  </si>
-  <si>
-    <t>Is Date Known: ${is_date_known}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Proxima Nova"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -731,110 +730,194 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="61">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,85 +926,32 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="FFEDEDED"/>
-      <rgbColor rgb="FFBDD7EE"/>
-      <rgbColor rgb="FFDEEBF7"/>
-      <rgbColor rgb="FFA9D18E"/>
-      <rgbColor rgb="FFE2F0D9"/>
-      <rgbColor rgb="FF2E75B6"/>
-      <rgbColor rgb="FFD0CECE"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffededed"/>
+      <rgbColor rgb="ffbdd7ee"/>
+      <rgbColor rgb="ffdeebf7"/>
+      <rgbColor rgb="ffa9d18e"/>
+      <rgbColor rgb="ffe2f0d9"/>
+      <rgbColor rgb="ff2e75b6"/>
+      <rgbColor rgb="ffd0cece"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1123,7 +1153,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1142,7 +1172,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1172,7 +1202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,7 +1228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1276,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1328,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,7 +1384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1380,7 +1410,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1393,15 +1423,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1418,7 +1442,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1437,7 +1461,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1463,7 +1487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1489,7 +1513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1515,7 +1539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1541,7 +1565,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1567,7 +1591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1593,7 +1617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1619,7 +1643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1645,7 +1669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1671,7 +1695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1684,15 +1708,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1706,7 +1724,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1725,7 +1743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1755,7 +1773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1781,7 +1799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1807,7 +1825,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1833,7 +1851,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1859,7 +1877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1885,7 +1903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1911,7 +1929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1937,7 +1955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1963,7 +1981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1976,84 +1994,75 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6719" style="1" customWidth="1"/>
     <col min="11" max="11" width="28.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="1" customWidth="1"/>
-    <col min="13" max="27" width="11.5" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.5" style="1"/>
+    <col min="12" max="12" width="12.8516" style="1" customWidth="1"/>
+    <col min="13" max="26" width="11.5" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" t="s" s="4">
         <v>11</v>
       </c>
       <c r="M1" s="5"/>
@@ -2071,20 +2080,20 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="15.25" customHeight="1">
+      <c r="A2" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s" s="10">
         <v>15</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" t="s" s="11">
         <v>16</v>
       </c>
       <c r="F2" s="12"/>
@@ -2109,25 +2118,25 @@
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
     </row>
-    <row r="3" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" ht="15.25" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" t="s" s="9">
         <v>19</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" t="s" s="11">
         <v>21</v>
       </c>
       <c r="K3" s="13"/>
@@ -2147,18 +2156,18 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" ht="15.25" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" t="s" s="9">
         <v>23</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F4" s="12"/>
@@ -2183,14 +2192,14 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A5" s="7" t="s">
+    <row r="5" ht="15.25" customHeight="1">
+      <c r="A5" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D5" s="12"/>
@@ -2217,26 +2226,26 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" ht="15.25" customHeight="1">
+      <c r="A6" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s" s="8">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" t="s" s="9">
         <v>28</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" t="s" s="10">
         <v>30</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="10" t="s">
+      <c r="I6" t="s" s="10">
         <v>31</v>
       </c>
       <c r="J6" s="12"/>
@@ -2257,14 +2266,14 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" ht="15.25" customHeight="1">
+      <c r="A7" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" t="s" s="9">
         <v>32</v>
       </c>
       <c r="D7" s="12"/>
@@ -2291,18 +2300,18 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" ht="15.25" customHeight="1">
+      <c r="A8" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s" s="9">
         <v>34</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F8" s="12"/>
@@ -2327,18 +2336,18 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" ht="15.25" customHeight="1">
+      <c r="A9" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" t="s" s="9">
         <v>36</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F9" s="12"/>
@@ -2363,14 +2372,14 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="10" ht="15.25" customHeight="1">
+      <c r="A10" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" t="s" s="9">
         <v>38</v>
       </c>
       <c r="D10" s="12"/>
@@ -2397,14 +2406,14 @@
       <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
     </row>
-    <row r="11" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A11" s="7" t="s">
+    <row r="11" ht="15.25" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s" s="8">
         <v>39</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s" s="9">
         <v>40</v>
       </c>
       <c r="D11" s="12"/>
@@ -2431,8 +2440,8 @@
       <c r="Y11" s="17"/>
       <c r="Z11" s="17"/>
     </row>
-    <row r="12" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A12" s="7" t="s">
+    <row r="12" ht="15.25" customHeight="1">
+      <c r="A12" t="s" s="7">
         <v>41</v>
       </c>
       <c r="B12" s="18"/>
@@ -2461,8 +2470,8 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
     </row>
-    <row r="13" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="13" ht="15.25" customHeight="1">
+      <c r="A13" t="s" s="7">
         <v>41</v>
       </c>
       <c r="B13" s="18"/>
@@ -2491,7 +2500,7 @@
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
     </row>
-    <row r="14" spans="1:26" ht="15.25" customHeight="1">
+    <row r="14" ht="15.25" customHeight="1">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2519,14 +2528,14 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A15" s="22" t="s">
+    <row r="15" ht="15.25" customHeight="1">
+      <c r="A15" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" t="s" s="23">
         <v>43</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" t="s" s="24">
         <v>32</v>
       </c>
       <c r="D15" s="25"/>
@@ -2536,7 +2545,7 @@
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="24" t="s">
+      <c r="K15" t="s" s="24">
         <v>44</v>
       </c>
       <c r="L15" s="26"/>
@@ -2555,14 +2564,14 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row r="16" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A16" s="22" t="s">
+    <row r="16" ht="15.25" customHeight="1">
+      <c r="A16" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" t="s" s="23">
         <v>45</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" t="s" s="24">
         <v>46</v>
       </c>
       <c r="D16" s="25"/>
@@ -2572,7 +2581,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="24" t="s">
+      <c r="K16" t="s" s="24">
         <v>47</v>
       </c>
       <c r="L16" s="26"/>
@@ -2591,14 +2600,14 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A17" s="22" t="s">
+    <row r="17" ht="15.25" customHeight="1">
+      <c r="A17" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" t="s" s="23">
         <v>48</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" t="s" s="24">
         <v>49</v>
       </c>
       <c r="D17" s="25"/>
@@ -2608,10 +2617,10 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="24" t="s">
+      <c r="K17" t="s" s="24">
         <v>50</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" t="s" s="24">
         <v>20</v>
       </c>
       <c r="M17" s="16"/>
@@ -2629,14 +2638,14 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A18" s="22" t="s">
+    <row r="18" ht="15.25" customHeight="1">
+      <c r="A18" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" t="s" s="23">
         <v>51</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" t="s" s="24">
         <v>52</v>
       </c>
       <c r="D18" s="25"/>
@@ -2646,7 +2655,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="24" t="s">
+      <c r="K18" t="s" s="24">
         <v>53</v>
       </c>
       <c r="L18" s="24"/>
@@ -2665,7 +2674,7 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row r="19" spans="1:26" ht="15.25" customHeight="1">
+    <row r="19" ht="15.25" customHeight="1">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -2693,19 +2702,19 @@
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
     </row>
-    <row r="20" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A20" s="27" t="s">
+    <row r="20" ht="29.25" customHeight="1">
+      <c r="A20" t="s" s="27">
         <v>54</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" t="s" s="28">
         <v>55</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" t="s" s="29">
         <v>56</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="31" t="s">
+      <c r="F20" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G20" s="30"/>
@@ -2729,21 +2738,21 @@
       <c r="Y20" s="17"/>
       <c r="Z20" s="17"/>
     </row>
-    <row r="21" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A21" s="27" t="s">
+    <row r="21" ht="29.25" customHeight="1">
+      <c r="A21" t="s" s="27">
         <v>17</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" t="s" s="28">
         <v>57</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" t="s" s="29">
         <v>58</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" t="s" s="31">
         <v>59</v>
       </c>
       <c r="E21" s="30"/>
-      <c r="F21" s="31" t="s">
+      <c r="F21" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G21" s="30"/>
@@ -2767,20 +2776,20 @@
       <c r="Y21" s="17"/>
       <c r="Z21" s="17"/>
     </row>
-    <row r="22" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A22" s="27" t="s">
+    <row r="22" ht="29.25" customHeight="1">
+      <c r="A22" t="s" s="27">
         <v>12</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" t="s" s="28">
         <v>60</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" t="s" s="29">
         <v>61</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" t="s" s="31">
         <v>62</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" t="s" s="31">
         <v>16</v>
       </c>
       <c r="F22" s="31"/>
@@ -2805,14 +2814,14 @@
       <c r="Y22" s="17"/>
       <c r="Z22" s="17"/>
     </row>
-    <row r="23" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A23" s="27" t="s">
+    <row r="23" ht="15.25" customHeight="1">
+      <c r="A23" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" t="s" s="28">
         <v>64</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" t="s" s="29">
         <v>65</v>
       </c>
       <c r="D23" s="31"/>
@@ -2839,19 +2848,19 @@
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
     </row>
-    <row r="24" spans="1:26" s="51" customFormat="1" ht="15.25" customHeight="1">
-      <c r="A24" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>133</v>
+    <row r="24" ht="15.25" customHeight="1">
+      <c r="A24" t="s" s="27">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s" s="28">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s" s="29">
+        <v>68</v>
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="31" t="s">
+      <c r="F24" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G24" s="30"/>
@@ -2875,25 +2884,29 @@
       <c r="Y24" s="17"/>
       <c r="Z24" s="17"/>
     </row>
-    <row r="25" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A25" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>134</v>
+    <row r="25" ht="15.25" customHeight="1">
+      <c r="A25" t="s" s="27">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s" s="28">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s" s="29">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s" s="31">
+        <v>72</v>
       </c>
       <c r="E25" s="30"/>
-      <c r="F25" s="31" t="s">
+      <c r="F25" t="s" s="31">
         <v>30</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
+      <c r="G25" t="s" s="31">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s" s="31">
+        <v>74</v>
+      </c>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
       <c r="K25" s="32"/>
@@ -2913,14 +2926,14 @@
       <c r="Y25" s="17"/>
       <c r="Z25" s="17"/>
     </row>
-    <row r="26" spans="1:26" ht="26.5" customHeight="1">
-      <c r="A26" s="27" t="s">
+    <row r="26" ht="26.5" customHeight="1">
+      <c r="A26" t="s" s="27">
         <v>42</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="29" t="s">
+      <c r="B26" t="s" s="28">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s" s="29">
         <v>61</v>
       </c>
       <c r="D26" s="31"/>
@@ -2930,8 +2943,8 @@
       <c r="H26" s="30"/>
       <c r="I26" s="30"/>
       <c r="J26" s="30"/>
-      <c r="K26" s="29" t="s">
-        <v>70</v>
+      <c r="K26" t="s" s="29">
+        <v>76</v>
       </c>
       <c r="L26" s="32"/>
       <c r="M26" s="16"/>
@@ -2949,8 +2962,8 @@
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A27" s="27" t="s">
+    <row r="27" ht="29.25" customHeight="1">
+      <c r="A27" t="s" s="27">
         <v>41</v>
       </c>
       <c r="B27" s="28"/>
@@ -2979,19 +2992,19 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A28" s="27" t="s">
+    <row r="28" ht="27.75" customHeight="1">
+      <c r="A28" t="s" s="27">
         <v>12</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>72</v>
+      <c r="B28" t="s" s="28">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D28" s="30"/>
-      <c r="E28" s="31" t="s">
-        <v>73</v>
+      <c r="E28" t="s" s="31">
+        <v>79</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
@@ -3015,19 +3028,19 @@
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A29" s="27" t="s">
+    <row r="29" ht="27.75" customHeight="1">
+      <c r="A29" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>75</v>
+      <c r="B29" t="s" s="28">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s" s="29">
+        <v>81</v>
       </c>
       <c r="D29" s="30"/>
-      <c r="E29" s="31" t="s">
-        <v>76</v>
+      <c r="E29" t="s" s="31">
+        <v>82</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -3051,19 +3064,19 @@
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A30" s="27" t="s">
+    <row r="30" ht="27.75" customHeight="1">
+      <c r="A30" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>78</v>
+      <c r="B30" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s" s="29">
+        <v>84</v>
       </c>
       <c r="D30" s="30"/>
-      <c r="E30" s="31" t="s">
-        <v>79</v>
+      <c r="E30" t="s" s="31">
+        <v>85</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
@@ -3087,15 +3100,15 @@
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
     </row>
-    <row r="31" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A31" s="27" t="s">
+    <row r="31" ht="27.75" customHeight="1">
+      <c r="A31" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>81</v>
+      <c r="B31" t="s" s="28">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s" s="29">
+        <v>87</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="31"/>
@@ -3121,19 +3134,19 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
     </row>
-    <row r="32" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A32" s="27" t="s">
+    <row r="32" ht="27.75" customHeight="1">
+      <c r="A32" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>83</v>
+      <c r="B32" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s" s="29">
+        <v>89</v>
       </c>
       <c r="D32" s="30"/>
-      <c r="E32" s="31" t="s">
-        <v>84</v>
+      <c r="E32" t="s" s="31">
+        <v>90</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
@@ -3157,15 +3170,15 @@
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
     </row>
-    <row r="33" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A33" s="27" t="s">
+    <row r="33" ht="15.25" customHeight="1">
+      <c r="A33" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>86</v>
+      <c r="B33" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s" s="33">
+        <v>92</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
@@ -3191,15 +3204,15 @@
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
     </row>
-    <row r="34" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A34" s="27" t="s">
+    <row r="34" ht="15.25" customHeight="1">
+      <c r="A34" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B34" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>88</v>
+      <c r="B34" t="s" s="28">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s" s="33">
+        <v>94</v>
       </c>
       <c r="D34" s="36"/>
       <c r="E34" s="36"/>
@@ -3225,15 +3238,15 @@
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
     </row>
-    <row r="35" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A35" s="27" t="s">
+    <row r="35" ht="15.25" customHeight="1">
+      <c r="A35" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>90</v>
+      <c r="B35" t="s" s="28">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s" s="33">
+        <v>96</v>
       </c>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -3259,15 +3272,15 @@
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
     </row>
-    <row r="36" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A36" s="27" t="s">
+    <row r="36" ht="15.25" customHeight="1">
+      <c r="A36" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>92</v>
+      <c r="B36" t="s" s="28">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s" s="33">
+        <v>98</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
@@ -3293,19 +3306,19 @@
       <c r="Y36" s="17"/>
       <c r="Z36" s="17"/>
     </row>
-    <row r="37" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A37" s="27" t="s">
+    <row r="37" ht="15.25" customHeight="1">
+      <c r="A37" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>94</v>
+      <c r="B37" t="s" s="28">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s" s="29">
+        <v>100</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="39" t="s">
-        <v>76</v>
+      <c r="E37" t="s" s="39">
+        <v>82</v>
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -3329,15 +3342,15 @@
       <c r="Y37" s="17"/>
       <c r="Z37" s="17"/>
     </row>
-    <row r="38" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A38" s="27" t="s">
+    <row r="38" ht="15.25" customHeight="1">
+      <c r="A38" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B38" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>96</v>
+      <c r="B38" t="s" s="41">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s" s="42">
+        <v>102</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -3363,25 +3376,25 @@
       <c r="Y38" s="17"/>
       <c r="Z38" s="17"/>
     </row>
-    <row r="39" spans="1:26" s="51" customFormat="1" ht="15.25" customHeight="1">
-      <c r="A39" s="27" t="s">
+    <row r="39" ht="15.25" customHeight="1">
+      <c r="A39" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B39" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
+      <c r="B39" t="s" s="43">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s" s="44">
+        <v>104</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
       <c r="M39" s="16"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17"/>
@@ -3397,18 +3410,18 @@
       <c r="Y39" s="17"/>
       <c r="Z39" s="17"/>
     </row>
-    <row r="40" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A40" s="27" t="s">
+    <row r="40" ht="15.25" customHeight="1">
+      <c r="A40" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B40" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>134</v>
+      <c r="B40" t="s" s="43">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s" s="46">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s" s="47">
+        <v>72</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="36"/>
@@ -3433,8 +3446,8 @@
       <c r="Y40" s="17"/>
       <c r="Z40" s="17"/>
     </row>
-    <row r="41" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A41" s="45" t="s">
+    <row r="41" ht="15.25" customHeight="1">
+      <c r="A41" t="s" s="48">
         <v>41</v>
       </c>
       <c r="B41" s="36"/>
@@ -3463,8 +3476,8 @@
       <c r="Y41" s="17"/>
       <c r="Z41" s="17"/>
     </row>
-    <row r="42" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A42" s="46"/>
+    <row r="42" ht="15.25" customHeight="1">
+      <c r="A42" s="49"/>
       <c r="B42" s="36"/>
       <c r="C42" s="37"/>
       <c r="D42" s="36"/>
@@ -3492,8 +3505,8 @@
       <c r="Z42" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3501,277 +3514,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="47" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="47" customWidth="1"/>
-    <col min="4" max="6" width="11.5" style="47" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="47"/>
+    <col min="1" max="1" width="16.5" style="50" customWidth="1"/>
+    <col min="2" max="2" width="20.6719" style="50" customWidth="1"/>
+    <col min="3" max="3" width="36.1719" style="50" customWidth="1"/>
+    <col min="4" max="5" width="11.5" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" ht="15.25" customHeight="1">
+      <c r="A1" t="s" s="51">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s" s="51">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" t="s" s="51">
         <v>2</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
-    <row r="2" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A2" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>101</v>
+    <row r="2" ht="15.25" customHeight="1">
+      <c r="A2" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s" s="53">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s" s="53">
+        <v>109</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A3" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>102</v>
+    <row r="3" ht="15.25" customHeight="1">
+      <c r="A3" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s" s="53">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s" s="53">
+        <v>110</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A4" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>103</v>
+    <row r="4" ht="15.25" customHeight="1">
+      <c r="A4" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s" s="53">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s" s="53">
+        <v>111</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A5" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>104</v>
+    <row r="5" ht="15.25" customHeight="1">
+      <c r="A5" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s" s="53">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s" s="53">
+        <v>112</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A6" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>105</v>
+    <row r="6" ht="15.25" customHeight="1">
+      <c r="A6" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s" s="53">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s" s="53">
+        <v>113</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A7" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>106</v>
+    <row r="7" ht="15.25" customHeight="1">
+      <c r="A7" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s" s="53">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s" s="53">
+        <v>114</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A8" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>107</v>
+    <row r="8" ht="15.25" customHeight="1">
+      <c r="A8" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s" s="53">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s" s="53">
+        <v>115</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A9" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="50" t="s">
+    <row r="9" ht="15.25" customHeight="1">
+      <c r="A9" t="s" s="52">
         <v>108</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>108</v>
+      <c r="B9" t="s" s="53">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s" s="53">
+        <v>116</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A10" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>109</v>
+    <row r="10" ht="15.25" customHeight="1">
+      <c r="A10" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s" s="53">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s" s="53">
+        <v>117</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A11" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>110</v>
+    <row r="11" ht="15.25" customHeight="1">
+      <c r="A11" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s" s="53">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s" s="53">
+        <v>118</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A12" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>111</v>
+    <row r="12" ht="15.25" customHeight="1">
+      <c r="A12" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s" s="53">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s" s="53">
+        <v>119</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A13" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>112</v>
+    <row r="13" ht="15.25" customHeight="1">
+      <c r="A13" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s" s="53">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s" s="53">
+        <v>120</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A14" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>113</v>
+    <row r="14" ht="15.25" customHeight="1">
+      <c r="A14" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s" s="53">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s" s="53">
+        <v>121</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A15" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>114</v>
+    <row r="15" ht="15.25" customHeight="1">
+      <c r="A15" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s" s="53">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s" s="53">
+        <v>122</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A16" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>115</v>
+    <row r="16" ht="15.25" customHeight="1">
+      <c r="A16" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s" s="53">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s" s="53">
+        <v>123</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A17" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>116</v>
+    <row r="17" ht="15.25" customHeight="1">
+      <c r="A17" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s" s="53">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s" s="53">
+        <v>124</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
     </row>
-    <row r="18" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A18" s="49"/>
+    <row r="18" ht="15.25" customHeight="1">
+      <c r="A18" s="52"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A19" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="58" t="s">
+    <row r="19" ht="15.25" customHeight="1">
+      <c r="A19" t="s" s="52">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s" s="53">
         <v>30</v>
       </c>
-      <c r="C19" s="58" t="s">
-        <v>135</v>
+      <c r="C19" t="s" s="53">
+        <v>125</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A20" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>136</v>
+    <row r="20" ht="15.25" customHeight="1">
+      <c r="A20" t="s" s="53">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s" s="53">
+        <v>126</v>
+      </c>
+      <c r="C20" t="s" s="53">
+        <v>127</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" ht="15.25" customHeight="1">
+    <row r="21" ht="15.25" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3779,8 +3790,8 @@
       <c r="E21" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3788,114 +3799,113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32" style="51" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="51" customWidth="1"/>
-    <col min="5" max="15" width="11.5" style="51" customWidth="1"/>
-    <col min="16" max="26" width="8.83203125" style="51" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="51" customWidth="1"/>
-    <col min="28" max="16384" width="11.5" style="51"/>
+    <col min="1" max="1" width="32" style="54" customWidth="1"/>
+    <col min="2" max="2" width="43.8516" style="54" customWidth="1"/>
+    <col min="3" max="3" width="32.8516" style="54" customWidth="1"/>
+    <col min="4" max="4" width="20.8516" style="54" customWidth="1"/>
+    <col min="5" max="15" width="11.5" style="54" customWidth="1"/>
+    <col min="16" max="26" width="8.85156" style="54" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" s="52" t="s">
+    <row r="1" ht="18" customHeight="1">
+      <c r="A1" t="s" s="55">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s" s="55">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s" s="55">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s" s="55">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s" s="55">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s" s="55">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s" s="55">
         <v>1</v>
       </c>
-      <c r="H1" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="56">
+      <c r="H1" t="s" s="55">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s" s="55">
+        <v>135</v>
+      </c>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s" s="57">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s" s="58">
+        <v>137</v>
+      </c>
+      <c r="C2" s="59">
         <v>43008</v>
       </c>
-      <c r="D2" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.25" customHeight="1">
+      <c r="D2" t="s" s="58">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s" s="58">
+        <v>139</v>
+      </c>
+      <c r="F2" s="60"/>
+      <c r="G2" t="s" s="58">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s" s="58">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s" s="58">
+        <v>141</v>
+      </c>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+    </row>
+    <row r="3" ht="15.25" customHeight="1">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -3923,7 +3933,7 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" ht="15.25" customHeight="1">
+    <row r="4" ht="15.25" customHeight="1">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -3951,7 +3961,7 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" spans="1:26" ht="15.25" customHeight="1">
+    <row r="5" ht="15.25" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -3979,7 +3989,7 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" spans="1:26" ht="15.25" customHeight="1">
+    <row r="6" ht="15.25" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -4007,7 +4017,7 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" ht="15.25" customHeight="1">
+    <row r="7" ht="15.25" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -4035,7 +4045,7 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" spans="1:26" ht="15.25" customHeight="1">
+    <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4063,7 +4073,7 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" ht="15.25" customHeight="1">
+    <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -4091,7 +4101,7 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" ht="15.25" customHeight="1">
+    <row r="10" ht="15.25" customHeight="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -4120,8 +4130,8 @@
       <c r="Z10" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
oubound modules flow ids changed for dev workspace (#382)
* feat: hint  and constraint on tracing date (#372)

* itech-malawi-config-direct-messages (#374)

* Itech malawi config direct messages dev (#375)

* itech-malawi-config-direct-messages

* addition of telegram

* setting sms gateway

* change-rapidpro-gateway-flow-id (#376)

* oubound modules flow ids changed for dev workspace

Co-authored-by: femi oni <freefony@gmail.com>
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/tracing_outcome.xlsx
+++ b/itech-malawi/forms/app/tracing_outcome.xlsx
@@ -1,28 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/itech-malawi/forms/app/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8456943-42C1-6D43-A09B-DE518BBEC31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="survey" sheetId="1" r:id="rId4"/>
+    <sheet name="choices" sheetId="2" r:id="rId5"/>
+    <sheet name="settings" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
   <si>
     <t>type</t>
   </si>
@@ -222,13 +213,31 @@
     <t>Outcome: ${b2c_outcome}</t>
   </si>
   <si>
+    <t>select_one is_date_known</t>
+  </si>
+  <si>
+    <t>is_date_known</t>
+  </si>
+  <si>
+    <t>Is Date Known</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
     <t>date_of_event</t>
   </si>
   <si>
-    <t>Date of Event</t>
+    <t>Actual or Estimated Date of Event</t>
+  </si>
+  <si>
+    <t>${is_date_known} = 'yes'</t>
+  </si>
+  <si>
+    <t>.&lt;=date(today())</t>
+  </si>
+  <si>
+    <t>Value must be current or previous date</t>
   </si>
   <si>
     <t>formatted_doe</t>
@@ -315,10 +324,16 @@
     <t>Back To Care Outcome: ${b2c_outcome}</t>
   </si>
   <si>
+    <t>_is_date_known</t>
+  </si>
+  <si>
+    <t>Is Date Known: ${is_date_known}</t>
+  </si>
+  <si>
     <t>_date_of_event</t>
   </si>
   <si>
-    <t>Date of Event: ${formatted_doe}</t>
+    <t>Actual or Estimated Date of Event: ${formatted_doe}</t>
   </si>
   <si>
     <t>list_name</t>
@@ -375,6 +390,15 @@
     <t>Other</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -415,85 +439,60 @@
   </si>
   <si>
     <t>en</t>
-  </si>
-  <si>
-    <t>is_date_known</t>
-  </si>
-  <si>
-    <t>select_one is_date_known</t>
-  </si>
-  <si>
-    <t>Is Date Known</t>
-  </si>
-  <si>
-    <t>${is_date_known} = 'yes'</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>_is_date_known</t>
-  </si>
-  <si>
-    <t>Is Date Known: ${is_date_known}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Proxima Nova"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -731,110 +730,194 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="61">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,85 +926,32 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="FFEDEDED"/>
-      <rgbColor rgb="FFBDD7EE"/>
-      <rgbColor rgb="FFDEEBF7"/>
-      <rgbColor rgb="FFA9D18E"/>
-      <rgbColor rgb="FFE2F0D9"/>
-      <rgbColor rgb="FF2E75B6"/>
-      <rgbColor rgb="FFD0CECE"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffededed"/>
+      <rgbColor rgb="ffbdd7ee"/>
+      <rgbColor rgb="ffdeebf7"/>
+      <rgbColor rgb="ffa9d18e"/>
+      <rgbColor rgb="ffe2f0d9"/>
+      <rgbColor rgb="ff2e75b6"/>
+      <rgbColor rgb="ffd0cece"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1123,7 +1153,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1142,7 +1172,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1172,7 +1202,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,7 +1228,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1254,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1280,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1276,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1328,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,7 +1384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1380,7 +1410,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1393,15 +1423,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1418,7 +1442,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1437,7 +1461,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1463,7 +1487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1489,7 +1513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1515,7 +1539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1541,7 +1565,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1567,7 +1591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1593,7 +1617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1619,7 +1643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1645,7 +1669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1671,7 +1695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1684,15 +1708,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1706,7 +1724,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1725,7 +1743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1755,7 +1773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1781,7 +1799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1807,7 +1825,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1833,7 +1851,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1859,7 +1877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1885,7 +1903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1911,7 +1929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1937,7 +1955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1963,7 +1981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1976,84 +1994,75 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6719" style="1" customWidth="1"/>
     <col min="11" max="11" width="28.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="1" customWidth="1"/>
-    <col min="13" max="27" width="11.5" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="11.5" style="1"/>
+    <col min="12" max="12" width="12.8516" style="1" customWidth="1"/>
+    <col min="13" max="26" width="11.5" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" t="s" s="4">
         <v>11</v>
       </c>
       <c r="M1" s="5"/>
@@ -2071,20 +2080,20 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="15.25" customHeight="1">
+      <c r="A2" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s" s="10">
         <v>15</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" t="s" s="11">
         <v>16</v>
       </c>
       <c r="F2" s="12"/>
@@ -2109,25 +2118,25 @@
       <c r="Y2" s="15"/>
       <c r="Z2" s="15"/>
     </row>
-    <row r="3" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" ht="15.25" customHeight="1">
+      <c r="A3" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" t="s" s="9">
         <v>19</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="11" t="s">
+      <c r="E3" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" t="s" s="11">
         <v>21</v>
       </c>
       <c r="K3" s="13"/>
@@ -2147,18 +2156,18 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" ht="15.25" customHeight="1">
+      <c r="A4" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" t="s" s="9">
         <v>23</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F4" s="12"/>
@@ -2183,14 +2192,14 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A5" s="7" t="s">
+    <row r="5" ht="15.25" customHeight="1">
+      <c r="A5" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D5" s="12"/>
@@ -2217,26 +2226,26 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" ht="15.25" customHeight="1">
+      <c r="A6" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s" s="8">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" t="s" s="9">
         <v>28</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" t="s" s="10">
         <v>30</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="10" t="s">
+      <c r="I6" t="s" s="10">
         <v>31</v>
       </c>
       <c r="J6" s="12"/>
@@ -2257,14 +2266,14 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" ht="15.25" customHeight="1">
+      <c r="A7" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" t="s" s="9">
         <v>32</v>
       </c>
       <c r="D7" s="12"/>
@@ -2291,18 +2300,18 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" ht="15.25" customHeight="1">
+      <c r="A8" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s" s="9">
         <v>34</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F8" s="12"/>
@@ -2327,18 +2336,18 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" ht="15.25" customHeight="1">
+      <c r="A9" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" t="s" s="9">
         <v>36</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" t="s" s="11">
         <v>20</v>
       </c>
       <c r="F9" s="12"/>
@@ -2363,14 +2372,14 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="10" ht="15.25" customHeight="1">
+      <c r="A10" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" t="s" s="9">
         <v>38</v>
       </c>
       <c r="D10" s="12"/>
@@ -2397,14 +2406,14 @@
       <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
     </row>
-    <row r="11" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A11" s="7" t="s">
+    <row r="11" ht="15.25" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s" s="8">
         <v>39</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s" s="9">
         <v>40</v>
       </c>
       <c r="D11" s="12"/>
@@ -2431,8 +2440,8 @@
       <c r="Y11" s="17"/>
       <c r="Z11" s="17"/>
     </row>
-    <row r="12" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A12" s="7" t="s">
+    <row r="12" ht="15.25" customHeight="1">
+      <c r="A12" t="s" s="7">
         <v>41</v>
       </c>
       <c r="B12" s="18"/>
@@ -2461,8 +2470,8 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
     </row>
-    <row r="13" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="13" ht="15.25" customHeight="1">
+      <c r="A13" t="s" s="7">
         <v>41</v>
       </c>
       <c r="B13" s="18"/>
@@ -2491,7 +2500,7 @@
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
     </row>
-    <row r="14" spans="1:26" ht="15.25" customHeight="1">
+    <row r="14" ht="15.25" customHeight="1">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -2519,14 +2528,14 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A15" s="22" t="s">
+    <row r="15" ht="15.25" customHeight="1">
+      <c r="A15" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" t="s" s="23">
         <v>43</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" t="s" s="24">
         <v>32</v>
       </c>
       <c r="D15" s="25"/>
@@ -2536,7 +2545,7 @@
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="24" t="s">
+      <c r="K15" t="s" s="24">
         <v>44</v>
       </c>
       <c r="L15" s="26"/>
@@ -2555,14 +2564,14 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row r="16" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A16" s="22" t="s">
+    <row r="16" ht="15.25" customHeight="1">
+      <c r="A16" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" t="s" s="23">
         <v>45</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" t="s" s="24">
         <v>46</v>
       </c>
       <c r="D16" s="25"/>
@@ -2572,7 +2581,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="24" t="s">
+      <c r="K16" t="s" s="24">
         <v>47</v>
       </c>
       <c r="L16" s="26"/>
@@ -2591,14 +2600,14 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A17" s="22" t="s">
+    <row r="17" ht="15.25" customHeight="1">
+      <c r="A17" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" t="s" s="23">
         <v>48</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" t="s" s="24">
         <v>49</v>
       </c>
       <c r="D17" s="25"/>
@@ -2608,10 +2617,10 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="24" t="s">
+      <c r="K17" t="s" s="24">
         <v>50</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" t="s" s="24">
         <v>20</v>
       </c>
       <c r="M17" s="16"/>
@@ -2629,14 +2638,14 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A18" s="22" t="s">
+    <row r="18" ht="15.25" customHeight="1">
+      <c r="A18" t="s" s="22">
         <v>42</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" t="s" s="23">
         <v>51</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" t="s" s="24">
         <v>52</v>
       </c>
       <c r="D18" s="25"/>
@@ -2646,7 +2655,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="24" t="s">
+      <c r="K18" t="s" s="24">
         <v>53</v>
       </c>
       <c r="L18" s="24"/>
@@ -2665,7 +2674,7 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row r="19" spans="1:26" ht="15.25" customHeight="1">
+    <row r="19" ht="15.25" customHeight="1">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -2693,19 +2702,19 @@
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
     </row>
-    <row r="20" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A20" s="27" t="s">
+    <row r="20" ht="29.25" customHeight="1">
+      <c r="A20" t="s" s="27">
         <v>54</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" t="s" s="28">
         <v>55</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" t="s" s="29">
         <v>56</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="31" t="s">
+      <c r="F20" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G20" s="30"/>
@@ -2729,21 +2738,21 @@
       <c r="Y20" s="17"/>
       <c r="Z20" s="17"/>
     </row>
-    <row r="21" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A21" s="27" t="s">
+    <row r="21" ht="29.25" customHeight="1">
+      <c r="A21" t="s" s="27">
         <v>17</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" t="s" s="28">
         <v>57</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" t="s" s="29">
         <v>58</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" t="s" s="31">
         <v>59</v>
       </c>
       <c r="E21" s="30"/>
-      <c r="F21" s="31" t="s">
+      <c r="F21" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G21" s="30"/>
@@ -2767,20 +2776,20 @@
       <c r="Y21" s="17"/>
       <c r="Z21" s="17"/>
     </row>
-    <row r="22" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A22" s="27" t="s">
+    <row r="22" ht="29.25" customHeight="1">
+      <c r="A22" t="s" s="27">
         <v>12</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" t="s" s="28">
         <v>60</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" t="s" s="29">
         <v>61</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" t="s" s="31">
         <v>62</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" t="s" s="31">
         <v>16</v>
       </c>
       <c r="F22" s="31"/>
@@ -2805,14 +2814,14 @@
       <c r="Y22" s="17"/>
       <c r="Z22" s="17"/>
     </row>
-    <row r="23" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A23" s="27" t="s">
+    <row r="23" ht="15.25" customHeight="1">
+      <c r="A23" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" t="s" s="28">
         <v>64</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" t="s" s="29">
         <v>65</v>
       </c>
       <c r="D23" s="31"/>
@@ -2839,19 +2848,19 @@
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
     </row>
-    <row r="24" spans="1:26" s="51" customFormat="1" ht="15.25" customHeight="1">
-      <c r="A24" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>133</v>
+    <row r="24" ht="15.25" customHeight="1">
+      <c r="A24" t="s" s="27">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s" s="28">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s" s="29">
+        <v>68</v>
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="31" t="s">
+      <c r="F24" t="s" s="31">
         <v>30</v>
       </c>
       <c r="G24" s="30"/>
@@ -2875,25 +2884,29 @@
       <c r="Y24" s="17"/>
       <c r="Z24" s="17"/>
     </row>
-    <row r="25" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A25" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>134</v>
+    <row r="25" ht="15.25" customHeight="1">
+      <c r="A25" t="s" s="27">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s" s="28">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s" s="29">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s" s="31">
+        <v>72</v>
       </c>
       <c r="E25" s="30"/>
-      <c r="F25" s="31" t="s">
+      <c r="F25" t="s" s="31">
         <v>30</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
+      <c r="G25" t="s" s="31">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s" s="31">
+        <v>74</v>
+      </c>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
       <c r="K25" s="32"/>
@@ -2913,14 +2926,14 @@
       <c r="Y25" s="17"/>
       <c r="Z25" s="17"/>
     </row>
-    <row r="26" spans="1:26" ht="26.5" customHeight="1">
-      <c r="A26" s="27" t="s">
+    <row r="26" ht="26.5" customHeight="1">
+      <c r="A26" t="s" s="27">
         <v>42</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="29" t="s">
+      <c r="B26" t="s" s="28">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s" s="29">
         <v>61</v>
       </c>
       <c r="D26" s="31"/>
@@ -2930,8 +2943,8 @@
       <c r="H26" s="30"/>
       <c r="I26" s="30"/>
       <c r="J26" s="30"/>
-      <c r="K26" s="29" t="s">
-        <v>70</v>
+      <c r="K26" t="s" s="29">
+        <v>76</v>
       </c>
       <c r="L26" s="32"/>
       <c r="M26" s="16"/>
@@ -2949,8 +2962,8 @@
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27" spans="1:26" ht="29.25" customHeight="1">
-      <c r="A27" s="27" t="s">
+    <row r="27" ht="29.25" customHeight="1">
+      <c r="A27" t="s" s="27">
         <v>41</v>
       </c>
       <c r="B27" s="28"/>
@@ -2979,19 +2992,19 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A28" s="27" t="s">
+    <row r="28" ht="27.75" customHeight="1">
+      <c r="A28" t="s" s="27">
         <v>12</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>72</v>
+      <c r="B28" t="s" s="28">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s" s="29">
+        <v>78</v>
       </c>
       <c r="D28" s="30"/>
-      <c r="E28" s="31" t="s">
-        <v>73</v>
+      <c r="E28" t="s" s="31">
+        <v>79</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
@@ -3015,19 +3028,19 @@
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A29" s="27" t="s">
+    <row r="29" ht="27.75" customHeight="1">
+      <c r="A29" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>75</v>
+      <c r="B29" t="s" s="28">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s" s="29">
+        <v>81</v>
       </c>
       <c r="D29" s="30"/>
-      <c r="E29" s="31" t="s">
-        <v>76</v>
+      <c r="E29" t="s" s="31">
+        <v>82</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -3051,19 +3064,19 @@
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A30" s="27" t="s">
+    <row r="30" ht="27.75" customHeight="1">
+      <c r="A30" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>78</v>
+      <c r="B30" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s" s="29">
+        <v>84</v>
       </c>
       <c r="D30" s="30"/>
-      <c r="E30" s="31" t="s">
-        <v>79</v>
+      <c r="E30" t="s" s="31">
+        <v>85</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
@@ -3087,15 +3100,15 @@
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
     </row>
-    <row r="31" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A31" s="27" t="s">
+    <row r="31" ht="27.75" customHeight="1">
+      <c r="A31" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>81</v>
+      <c r="B31" t="s" s="28">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s" s="29">
+        <v>87</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="31"/>
@@ -3121,19 +3134,19 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
     </row>
-    <row r="32" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A32" s="27" t="s">
+    <row r="32" ht="27.75" customHeight="1">
+      <c r="A32" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>83</v>
+      <c r="B32" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s" s="29">
+        <v>89</v>
       </c>
       <c r="D32" s="30"/>
-      <c r="E32" s="31" t="s">
-        <v>84</v>
+      <c r="E32" t="s" s="31">
+        <v>90</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
@@ -3157,15 +3170,15 @@
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
     </row>
-    <row r="33" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A33" s="27" t="s">
+    <row r="33" ht="15.25" customHeight="1">
+      <c r="A33" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>86</v>
+      <c r="B33" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s" s="33">
+        <v>92</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
@@ -3191,15 +3204,15 @@
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
     </row>
-    <row r="34" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A34" s="27" t="s">
+    <row r="34" ht="15.25" customHeight="1">
+      <c r="A34" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B34" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>88</v>
+      <c r="B34" t="s" s="28">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s" s="33">
+        <v>94</v>
       </c>
       <c r="D34" s="36"/>
       <c r="E34" s="36"/>
@@ -3225,15 +3238,15 @@
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
     </row>
-    <row r="35" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A35" s="27" t="s">
+    <row r="35" ht="15.25" customHeight="1">
+      <c r="A35" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>90</v>
+      <c r="B35" t="s" s="28">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s" s="33">
+        <v>96</v>
       </c>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -3259,15 +3272,15 @@
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
     </row>
-    <row r="36" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A36" s="27" t="s">
+    <row r="36" ht="15.25" customHeight="1">
+      <c r="A36" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>92</v>
+      <c r="B36" t="s" s="28">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s" s="33">
+        <v>98</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
@@ -3293,19 +3306,19 @@
       <c r="Y36" s="17"/>
       <c r="Z36" s="17"/>
     </row>
-    <row r="37" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A37" s="27" t="s">
+    <row r="37" ht="15.25" customHeight="1">
+      <c r="A37" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>94</v>
+      <c r="B37" t="s" s="28">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s" s="29">
+        <v>100</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="39" t="s">
-        <v>76</v>
+      <c r="E37" t="s" s="39">
+        <v>82</v>
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -3329,15 +3342,15 @@
       <c r="Y37" s="17"/>
       <c r="Z37" s="17"/>
     </row>
-    <row r="38" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A38" s="27" t="s">
+    <row r="38" ht="15.25" customHeight="1">
+      <c r="A38" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B38" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>96</v>
+      <c r="B38" t="s" s="41">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s" s="42">
+        <v>102</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -3363,25 +3376,25 @@
       <c r="Y38" s="17"/>
       <c r="Z38" s="17"/>
     </row>
-    <row r="39" spans="1:26" s="51" customFormat="1" ht="15.25" customHeight="1">
-      <c r="A39" s="27" t="s">
+    <row r="39" ht="15.25" customHeight="1">
+      <c r="A39" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B39" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
+      <c r="B39" t="s" s="43">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s" s="44">
+        <v>104</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
       <c r="M39" s="16"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17"/>
@@ -3397,18 +3410,18 @@
       <c r="Y39" s="17"/>
       <c r="Z39" s="17"/>
     </row>
-    <row r="40" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A40" s="27" t="s">
+    <row r="40" ht="15.25" customHeight="1">
+      <c r="A40" t="s" s="27">
         <v>63</v>
       </c>
-      <c r="B40" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>134</v>
+      <c r="B40" t="s" s="43">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s" s="46">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s" s="47">
+        <v>72</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="36"/>
@@ -3433,8 +3446,8 @@
       <c r="Y40" s="17"/>
       <c r="Z40" s="17"/>
     </row>
-    <row r="41" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A41" s="45" t="s">
+    <row r="41" ht="15.25" customHeight="1">
+      <c r="A41" t="s" s="48">
         <v>41</v>
       </c>
       <c r="B41" s="36"/>
@@ -3463,8 +3476,8 @@
       <c r="Y41" s="17"/>
       <c r="Z41" s="17"/>
     </row>
-    <row r="42" spans="1:26" ht="15.25" customHeight="1">
-      <c r="A42" s="46"/>
+    <row r="42" ht="15.25" customHeight="1">
+      <c r="A42" s="49"/>
       <c r="B42" s="36"/>
       <c r="C42" s="37"/>
       <c r="D42" s="36"/>
@@ -3492,8 +3505,8 @@
       <c r="Z42" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3501,277 +3514,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="47" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="47" customWidth="1"/>
-    <col min="4" max="6" width="11.5" style="47" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="47"/>
+    <col min="1" max="1" width="16.5" style="50" customWidth="1"/>
+    <col min="2" max="2" width="20.6719" style="50" customWidth="1"/>
+    <col min="3" max="3" width="36.1719" style="50" customWidth="1"/>
+    <col min="4" max="5" width="11.5" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" ht="15.25" customHeight="1">
+      <c r="A1" t="s" s="51">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s" s="51">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" t="s" s="51">
         <v>2</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
-    <row r="2" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A2" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>101</v>
+    <row r="2" ht="15.25" customHeight="1">
+      <c r="A2" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s" s="53">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s" s="53">
+        <v>109</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A3" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>102</v>
+    <row r="3" ht="15.25" customHeight="1">
+      <c r="A3" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s" s="53">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s" s="53">
+        <v>110</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A4" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>103</v>
+    <row r="4" ht="15.25" customHeight="1">
+      <c r="A4" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s" s="53">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s" s="53">
+        <v>111</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A5" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>104</v>
+    <row r="5" ht="15.25" customHeight="1">
+      <c r="A5" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s" s="53">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s" s="53">
+        <v>112</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A6" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>105</v>
+    <row r="6" ht="15.25" customHeight="1">
+      <c r="A6" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s" s="53">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s" s="53">
+        <v>113</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A7" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>106</v>
+    <row r="7" ht="15.25" customHeight="1">
+      <c r="A7" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s" s="53">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s" s="53">
+        <v>114</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A8" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>107</v>
+    <row r="8" ht="15.25" customHeight="1">
+      <c r="A8" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s" s="53">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s" s="53">
+        <v>115</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A9" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="50" t="s">
+    <row r="9" ht="15.25" customHeight="1">
+      <c r="A9" t="s" s="52">
         <v>108</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>108</v>
+      <c r="B9" t="s" s="53">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s" s="53">
+        <v>116</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A10" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>109</v>
+    <row r="10" ht="15.25" customHeight="1">
+      <c r="A10" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s" s="53">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s" s="53">
+        <v>117</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A11" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>110</v>
+    <row r="11" ht="15.25" customHeight="1">
+      <c r="A11" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s" s="53">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s" s="53">
+        <v>118</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A12" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>111</v>
+    <row r="12" ht="15.25" customHeight="1">
+      <c r="A12" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s" s="53">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s" s="53">
+        <v>119</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A13" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>112</v>
+    <row r="13" ht="15.25" customHeight="1">
+      <c r="A13" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s" s="53">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s" s="53">
+        <v>120</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A14" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>113</v>
+    <row r="14" ht="15.25" customHeight="1">
+      <c r="A14" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s" s="53">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s" s="53">
+        <v>121</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A15" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>114</v>
+    <row r="15" ht="15.25" customHeight="1">
+      <c r="A15" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s" s="53">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s" s="53">
+        <v>122</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
-    <row r="16" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A16" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>115</v>
+    <row r="16" ht="15.25" customHeight="1">
+      <c r="A16" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s" s="53">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s" s="53">
+        <v>123</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A17" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>116</v>
+    <row r="17" ht="15.25" customHeight="1">
+      <c r="A17" t="s" s="52">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s" s="53">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s" s="53">
+        <v>124</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
     </row>
-    <row r="18" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A18" s="49"/>
+    <row r="18" ht="15.25" customHeight="1">
+      <c r="A18" s="52"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A19" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="58" t="s">
+    <row r="19" ht="15.25" customHeight="1">
+      <c r="A19" t="s" s="52">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s" s="53">
         <v>30</v>
       </c>
-      <c r="C19" s="58" t="s">
-        <v>135</v>
+      <c r="C19" t="s" s="53">
+        <v>125</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:5" ht="15.25" customHeight="1">
-      <c r="A20" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>136</v>
+    <row r="20" ht="15.25" customHeight="1">
+      <c r="A20" t="s" s="53">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s" s="53">
+        <v>126</v>
+      </c>
+      <c r="C20" t="s" s="53">
+        <v>127</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" ht="15.25" customHeight="1">
+    <row r="21" ht="15.25" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3779,8 +3790,8 @@
       <c r="E21" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3788,114 +3799,113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32" style="51" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="51" customWidth="1"/>
-    <col min="5" max="15" width="11.5" style="51" customWidth="1"/>
-    <col min="16" max="26" width="8.83203125" style="51" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="51" customWidth="1"/>
-    <col min="28" max="16384" width="11.5" style="51"/>
+    <col min="1" max="1" width="32" style="54" customWidth="1"/>
+    <col min="2" max="2" width="43.8516" style="54" customWidth="1"/>
+    <col min="3" max="3" width="32.8516" style="54" customWidth="1"/>
+    <col min="4" max="4" width="20.8516" style="54" customWidth="1"/>
+    <col min="5" max="15" width="11.5" style="54" customWidth="1"/>
+    <col min="16" max="26" width="8.85156" style="54" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" s="52" t="s">
+    <row r="1" ht="18" customHeight="1">
+      <c r="A1" t="s" s="55">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s" s="55">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s" s="55">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s" s="55">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s" s="55">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s" s="55">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s" s="55">
         <v>1</v>
       </c>
-      <c r="H1" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="56">
+      <c r="H1" t="s" s="55">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s" s="55">
+        <v>135</v>
+      </c>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s" s="57">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s" s="58">
+        <v>137</v>
+      </c>
+      <c r="C2" s="59">
         <v>43008</v>
       </c>
-      <c r="D2" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.25" customHeight="1">
+      <c r="D2" t="s" s="58">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s" s="58">
+        <v>139</v>
+      </c>
+      <c r="F2" s="60"/>
+      <c r="G2" t="s" s="58">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s" s="58">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s" s="58">
+        <v>141</v>
+      </c>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+    </row>
+    <row r="3" ht="15.25" customHeight="1">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -3923,7 +3933,7 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" ht="15.25" customHeight="1">
+    <row r="4" ht="15.25" customHeight="1">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -3951,7 +3961,7 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" spans="1:26" ht="15.25" customHeight="1">
+    <row r="5" ht="15.25" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -3979,7 +3989,7 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" spans="1:26" ht="15.25" customHeight="1">
+    <row r="6" ht="15.25" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -4007,7 +4017,7 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" ht="15.25" customHeight="1">
+    <row r="7" ht="15.25" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -4035,7 +4045,7 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" spans="1:26" ht="15.25" customHeight="1">
+    <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4063,7 +4073,7 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" ht="15.25" customHeight="1">
+    <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -4091,7 +4101,7 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" ht="15.25" customHeight="1">
+    <row r="10" ht="15.25" customHeight="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -4120,8 +4130,8 @@
       <c r="Z10" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>